<commit_message>
modified:   NBA2324.xlsx modified:   accuracy.ipynb modified:   future.xlsx modified:   nba_forecast.ipynb
</commit_message>
<xml_diff>
--- a/NBA2324.xlsx
+++ b/NBA2324.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkdb\OneDrive\Desktop\ballgorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554754A6-2243-4B60-8D79-FA7D7A9DC676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9604D1-FA74-40F4-B49E-B5891D2E521C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4029" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4089" uniqueCount="75">
   <si>
     <t>Attend.</t>
   </si>
@@ -592,9 +592,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I671"/>
+  <dimension ref="A1:I681"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A649" workbookViewId="0">
+      <selection activeCell="A681" sqref="A681"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -20067,6 +20069,296 @@
         <v>41</v>
       </c>
     </row>
+    <row r="672" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A672" t="s">
+        <v>14</v>
+      </c>
+      <c r="B672" s="3">
+        <v>118</v>
+      </c>
+      <c r="C672" t="s">
+        <v>20</v>
+      </c>
+      <c r="D672" s="3">
+        <v>104</v>
+      </c>
+      <c r="E672" t="s">
+        <v>67</v>
+      </c>
+      <c r="F672">
+        <v>17832</v>
+      </c>
+      <c r="G672" t="s">
+        <v>54</v>
+      </c>
+      <c r="H672" t="s">
+        <v>14</v>
+      </c>
+      <c r="I672" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="673" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A673" t="s">
+        <v>21</v>
+      </c>
+      <c r="B673" s="3">
+        <v>109</v>
+      </c>
+      <c r="C673" t="s">
+        <v>12</v>
+      </c>
+      <c r="D673" s="3">
+        <v>125</v>
+      </c>
+      <c r="E673" t="s">
+        <v>67</v>
+      </c>
+      <c r="F673">
+        <v>17832</v>
+      </c>
+      <c r="G673" t="s">
+        <v>13</v>
+      </c>
+      <c r="H673" t="s">
+        <v>12</v>
+      </c>
+      <c r="I673" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="674" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A674" t="s">
+        <v>44</v>
+      </c>
+      <c r="B674" s="3">
+        <v>105</v>
+      </c>
+      <c r="C674" t="s">
+        <v>3</v>
+      </c>
+      <c r="D674" s="3">
+        <v>111</v>
+      </c>
+      <c r="E674" t="s">
+        <v>67</v>
+      </c>
+      <c r="F674">
+        <v>17832</v>
+      </c>
+      <c r="G674" t="s">
+        <v>4</v>
+      </c>
+      <c r="H674" t="s">
+        <v>3</v>
+      </c>
+      <c r="I674" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="675" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A675" t="s">
+        <v>8</v>
+      </c>
+      <c r="B675" s="3">
+        <v>104</v>
+      </c>
+      <c r="C675" t="s">
+        <v>27</v>
+      </c>
+      <c r="D675" s="3">
+        <v>106</v>
+      </c>
+      <c r="E675" t="s">
+        <v>67</v>
+      </c>
+      <c r="F675">
+        <v>17832</v>
+      </c>
+      <c r="G675" t="s">
+        <v>28</v>
+      </c>
+      <c r="H675" t="s">
+        <v>27</v>
+      </c>
+      <c r="I675" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="676" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A676" t="s">
+        <v>42</v>
+      </c>
+      <c r="B676" s="3">
+        <v>115</v>
+      </c>
+      <c r="C676" t="s">
+        <v>11</v>
+      </c>
+      <c r="D676" s="3">
+        <v>96</v>
+      </c>
+      <c r="E676" t="s">
+        <v>67</v>
+      </c>
+      <c r="F676">
+        <v>17832</v>
+      </c>
+      <c r="G676" t="s">
+        <v>49</v>
+      </c>
+      <c r="H676" t="s">
+        <v>42</v>
+      </c>
+      <c r="I676" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="677" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A677" t="s">
+        <v>36</v>
+      </c>
+      <c r="B677" s="3">
+        <v>134</v>
+      </c>
+      <c r="C677" t="s">
+        <v>18</v>
+      </c>
+      <c r="D677" s="3">
+        <v>122</v>
+      </c>
+      <c r="E677" t="s">
+        <v>67</v>
+      </c>
+      <c r="F677">
+        <v>17832</v>
+      </c>
+      <c r="G677" t="s">
+        <v>19</v>
+      </c>
+      <c r="H677" t="s">
+        <v>36</v>
+      </c>
+      <c r="I677" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="678" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A678" t="s">
+        <v>29</v>
+      </c>
+      <c r="B678" s="3">
+        <v>117</v>
+      </c>
+      <c r="C678" t="s">
+        <v>45</v>
+      </c>
+      <c r="D678" s="3">
+        <v>141</v>
+      </c>
+      <c r="E678" t="s">
+        <v>67</v>
+      </c>
+      <c r="F678">
+        <v>17832</v>
+      </c>
+      <c r="G678" t="s">
+        <v>46</v>
+      </c>
+      <c r="H678" t="s">
+        <v>45</v>
+      </c>
+      <c r="I678" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="679" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A679" t="s">
+        <v>2</v>
+      </c>
+      <c r="B679" s="3">
+        <v>145</v>
+      </c>
+      <c r="C679" t="s">
+        <v>6</v>
+      </c>
+      <c r="D679" s="3">
+        <v>144</v>
+      </c>
+      <c r="E679" t="s">
+        <v>63</v>
+      </c>
+      <c r="F679">
+        <v>17832</v>
+      </c>
+      <c r="G679" t="s">
+        <v>7</v>
+      </c>
+      <c r="H679" t="s">
+        <v>2</v>
+      </c>
+      <c r="I679" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="680" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A680" t="s">
+        <v>23</v>
+      </c>
+      <c r="B680" s="3">
+        <v>112</v>
+      </c>
+      <c r="C680" t="s">
+        <v>39</v>
+      </c>
+      <c r="D680" s="3">
+        <v>113</v>
+      </c>
+      <c r="E680" t="s">
+        <v>67</v>
+      </c>
+      <c r="F680">
+        <v>17832</v>
+      </c>
+      <c r="G680" t="s">
+        <v>40</v>
+      </c>
+      <c r="H680" t="s">
+        <v>39</v>
+      </c>
+      <c r="I680" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="681" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A681" t="s">
+        <v>35</v>
+      </c>
+      <c r="B681" s="3">
+        <v>120</v>
+      </c>
+      <c r="C681" t="s">
+        <v>38</v>
+      </c>
+      <c r="D681" s="3">
+        <v>115</v>
+      </c>
+      <c r="E681" t="s">
+        <v>67</v>
+      </c>
+      <c r="F681">
+        <v>17832</v>
+      </c>
+      <c r="G681" t="s">
+        <v>51</v>
+      </c>
+      <c r="H681" t="s">
+        <v>35</v>
+      </c>
+      <c r="I681" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified:   NBA2324.xlsx modified:   future.xlsx modified:   nba_forecast.ipynb new file:   test_nba_forecast.ipynb
</commit_message>
<xml_diff>
--- a/NBA2324.xlsx
+++ b/NBA2324.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkdb\OneDrive\Desktop\ballgorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9863FE-62CB-49CF-B2CA-D6EEC5378939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0211C54-20B9-491E-9EE7-1E4FDEAE0C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4305" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4365" uniqueCount="75">
   <si>
     <t>Attend.</t>
   </si>
@@ -592,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I717"/>
+  <dimension ref="A1:I727"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A684" workbookViewId="0">
-      <selection activeCell="G714" sqref="G714"/>
+    <sheetView tabSelected="1" topLeftCell="A694" workbookViewId="0">
+      <selection activeCell="H719" sqref="H719"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -21403,6 +21403,296 @@
         <v>36</v>
       </c>
     </row>
+    <row r="718" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A718" t="s">
+        <v>42</v>
+      </c>
+      <c r="B718" s="3">
+        <v>136</v>
+      </c>
+      <c r="C718" t="s">
+        <v>20</v>
+      </c>
+      <c r="D718" s="3">
+        <v>125</v>
+      </c>
+      <c r="E718" t="s">
+        <v>67</v>
+      </c>
+      <c r="F718">
+        <v>17832</v>
+      </c>
+      <c r="G718" t="s">
+        <v>54</v>
+      </c>
+      <c r="H718" t="s">
+        <v>42</v>
+      </c>
+      <c r="I718" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="719" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A719" t="s">
+        <v>21</v>
+      </c>
+      <c r="B719" s="3">
+        <v>110</v>
+      </c>
+      <c r="C719" t="s">
+        <v>14</v>
+      </c>
+      <c r="D719" s="3">
+        <v>102</v>
+      </c>
+      <c r="E719" t="s">
+        <v>67</v>
+      </c>
+      <c r="F719">
+        <v>17832</v>
+      </c>
+      <c r="G719" t="s">
+        <v>55</v>
+      </c>
+      <c r="H719" t="s">
+        <v>21</v>
+      </c>
+      <c r="I719" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="720" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A720" t="s">
+        <v>5</v>
+      </c>
+      <c r="B720" s="3">
+        <v>120</v>
+      </c>
+      <c r="C720" t="s">
+        <v>17</v>
+      </c>
+      <c r="D720" s="3">
+        <v>129</v>
+      </c>
+      <c r="E720" t="s">
+        <v>67</v>
+      </c>
+      <c r="F720">
+        <v>17832</v>
+      </c>
+      <c r="G720" t="s">
+        <v>47</v>
+      </c>
+      <c r="H720" t="s">
+        <v>17</v>
+      </c>
+      <c r="I720" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="721" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A721" t="s">
+        <v>35</v>
+      </c>
+      <c r="B721" s="3">
+        <v>133</v>
+      </c>
+      <c r="C721" t="s">
+        <v>15</v>
+      </c>
+      <c r="D721" s="3">
+        <v>122</v>
+      </c>
+      <c r="E721" t="s">
+        <v>67</v>
+      </c>
+      <c r="F721">
+        <v>17832</v>
+      </c>
+      <c r="G721" t="s">
+        <v>16</v>
+      </c>
+      <c r="H721" t="s">
+        <v>35</v>
+      </c>
+      <c r="I721" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="722" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A722" t="s">
+        <v>24</v>
+      </c>
+      <c r="B722" s="3">
+        <v>106</v>
+      </c>
+      <c r="C722" t="s">
+        <v>8</v>
+      </c>
+      <c r="D722" s="3">
+        <v>135</v>
+      </c>
+      <c r="E722" t="s">
+        <v>67</v>
+      </c>
+      <c r="F722">
+        <v>17832</v>
+      </c>
+      <c r="G722" t="s">
+        <v>60</v>
+      </c>
+      <c r="H722" t="s">
+        <v>8</v>
+      </c>
+      <c r="I722" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="723" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A723" t="s">
+        <v>6</v>
+      </c>
+      <c r="B723" s="3">
+        <v>121</v>
+      </c>
+      <c r="C723" t="s">
+        <v>30</v>
+      </c>
+      <c r="D723" s="3">
+        <v>101</v>
+      </c>
+      <c r="E723" t="s">
+        <v>67</v>
+      </c>
+      <c r="F723">
+        <v>17832</v>
+      </c>
+      <c r="G723" t="s">
+        <v>31</v>
+      </c>
+      <c r="H723" t="s">
+        <v>6</v>
+      </c>
+      <c r="I723" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="724" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A724" t="s">
+        <v>9</v>
+      </c>
+      <c r="B724" s="3">
+        <v>108</v>
+      </c>
+      <c r="C724" t="s">
+        <v>23</v>
+      </c>
+      <c r="D724" s="3">
+        <v>106</v>
+      </c>
+      <c r="E724" t="s">
+        <v>67</v>
+      </c>
+      <c r="F724">
+        <v>17832</v>
+      </c>
+      <c r="G724" t="s">
+        <v>57</v>
+      </c>
+      <c r="H724" t="s">
+        <v>9</v>
+      </c>
+      <c r="I724" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="725" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A725" t="s">
+        <v>18</v>
+      </c>
+      <c r="B725" s="3">
+        <v>106</v>
+      </c>
+      <c r="C725" t="s">
+        <v>32</v>
+      </c>
+      <c r="D725" s="3">
+        <v>126</v>
+      </c>
+      <c r="E725" t="s">
+        <v>67</v>
+      </c>
+      <c r="F725">
+        <v>17832</v>
+      </c>
+      <c r="G725" t="s">
+        <v>59</v>
+      </c>
+      <c r="H725" t="s">
+        <v>32</v>
+      </c>
+      <c r="I725" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="726" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A726" t="s">
+        <v>29</v>
+      </c>
+      <c r="B726" s="3">
+        <v>114</v>
+      </c>
+      <c r="C726" t="s">
+        <v>39</v>
+      </c>
+      <c r="D726" s="3">
+        <v>113</v>
+      </c>
+      <c r="E726" t="s">
+        <v>67</v>
+      </c>
+      <c r="F726">
+        <v>17832</v>
+      </c>
+      <c r="G726" t="s">
+        <v>40</v>
+      </c>
+      <c r="H726" t="s">
+        <v>29</v>
+      </c>
+      <c r="I726" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="727" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A727" t="s">
+        <v>41</v>
+      </c>
+      <c r="B727" s="3">
+        <v>108</v>
+      </c>
+      <c r="C727" t="s">
+        <v>3</v>
+      </c>
+      <c r="D727" s="3">
+        <v>120</v>
+      </c>
+      <c r="E727" t="s">
+        <v>67</v>
+      </c>
+      <c r="F727">
+        <v>17832</v>
+      </c>
+      <c r="G727" t="s">
+        <v>4</v>
+      </c>
+      <c r="H727" t="s">
+        <v>3</v>
+      </c>
+      <c r="I727" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified:   NBA2324.xlsx new file:   cumulative_accuracy.ipynb new file:   espn_comparison.ipynb new file:   espn_comparison.xlsx modified:   future.xlsx modified:   nba_forecast.ipynb modified:   nba_v1.1.ipynb
</commit_message>
<xml_diff>
--- a/NBA2324.xlsx
+++ b/NBA2324.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkdb\OneDrive\Desktop\ballgorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0211C54-20B9-491E-9EE7-1E4FDEAE0C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E68233-CC05-4DC2-9208-1147D53B2E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4365" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4401" uniqueCount="75">
   <si>
     <t>Attend.</t>
   </si>
@@ -592,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I727"/>
+  <dimension ref="A1:I733"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A694" workbookViewId="0">
-      <selection activeCell="H719" sqref="H719"/>
+    <sheetView tabSelected="1" topLeftCell="A701" workbookViewId="0">
+      <selection activeCell="A728" sqref="A728"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -21693,6 +21693,180 @@
         <v>41</v>
       </c>
     </row>
+    <row r="728" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A728" t="s">
+        <v>27</v>
+      </c>
+      <c r="B728" s="3">
+        <v>136</v>
+      </c>
+      <c r="C728" t="s">
+        <v>44</v>
+      </c>
+      <c r="D728" s="3">
+        <v>121</v>
+      </c>
+      <c r="E728" t="s">
+        <v>67</v>
+      </c>
+      <c r="F728">
+        <v>17832</v>
+      </c>
+      <c r="G728" t="s">
+        <v>61</v>
+      </c>
+      <c r="H728" t="s">
+        <v>27</v>
+      </c>
+      <c r="I728" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="729" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A729" t="s">
+        <v>6</v>
+      </c>
+      <c r="B729" s="3">
+        <v>134</v>
+      </c>
+      <c r="C729" t="s">
+        <v>17</v>
+      </c>
+      <c r="D729" s="3">
+        <v>141</v>
+      </c>
+      <c r="E729" t="s">
+        <v>50</v>
+      </c>
+      <c r="F729">
+        <v>17832</v>
+      </c>
+      <c r="G729" t="s">
+        <v>47</v>
+      </c>
+      <c r="H729" t="s">
+        <v>17</v>
+      </c>
+      <c r="I729" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="730" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A730" t="s">
+        <v>35</v>
+      </c>
+      <c r="B730" s="3">
+        <v>123</v>
+      </c>
+      <c r="C730" t="s">
+        <v>33</v>
+      </c>
+      <c r="D730" s="3">
+        <v>115</v>
+      </c>
+      <c r="E730" t="s">
+        <v>67</v>
+      </c>
+      <c r="F730">
+        <v>17832</v>
+      </c>
+      <c r="G730" t="s">
+        <v>34</v>
+      </c>
+      <c r="H730" t="s">
+        <v>35</v>
+      </c>
+      <c r="I730" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="731" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A731" t="s">
+        <v>45</v>
+      </c>
+      <c r="B731" s="3">
+        <v>129</v>
+      </c>
+      <c r="C731" t="s">
+        <v>38</v>
+      </c>
+      <c r="D731" s="3">
+        <v>117</v>
+      </c>
+      <c r="E731" t="s">
+        <v>67</v>
+      </c>
+      <c r="F731">
+        <v>17832</v>
+      </c>
+      <c r="G731" t="s">
+        <v>51</v>
+      </c>
+      <c r="H731" t="s">
+        <v>45</v>
+      </c>
+      <c r="I731" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="732" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A732" t="s">
+        <v>2</v>
+      </c>
+      <c r="B732" s="3">
+        <v>113</v>
+      </c>
+      <c r="C732" t="s">
+        <v>12</v>
+      </c>
+      <c r="D732" s="3">
+        <v>105</v>
+      </c>
+      <c r="E732" t="s">
+        <v>67</v>
+      </c>
+      <c r="F732">
+        <v>17832</v>
+      </c>
+      <c r="G732" t="s">
+        <v>13</v>
+      </c>
+      <c r="H732" t="s">
+        <v>2</v>
+      </c>
+      <c r="I732" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="733" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A733" t="s">
+        <v>26</v>
+      </c>
+      <c r="B733" s="3">
+        <v>117</v>
+      </c>
+      <c r="C733" t="s">
+        <v>39</v>
+      </c>
+      <c r="D733" s="3">
+        <v>101</v>
+      </c>
+      <c r="E733" t="s">
+        <v>67</v>
+      </c>
+      <c r="F733">
+        <v>17832</v>
+      </c>
+      <c r="G733" t="s">
+        <v>40</v>
+      </c>
+      <c r="H733" t="s">
+        <v>26</v>
+      </c>
+      <c r="I733" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified:   NBA2324.xlsx modified:   cumulative_accuracy.ipynb modified:   espn_comparison.ipynb modified:   espn_comparison.xlsx modified:   future.xlsx modified:   nba_v1.1.ipynb
</commit_message>
<xml_diff>
--- a/NBA2324.xlsx
+++ b/NBA2324.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkdb\OneDrive\Desktop\ballgorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E68233-CC05-4DC2-9208-1147D53B2E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5C706B-CB2E-43F8-811C-44E837A6EFFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4401" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4455" uniqueCount="75">
   <si>
     <t>Attend.</t>
   </si>
@@ -592,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I733"/>
+  <dimension ref="A1:I742"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A701" workbookViewId="0">
-      <selection activeCell="A728" sqref="A728"/>
+    <sheetView tabSelected="1" topLeftCell="A709" workbookViewId="0">
+      <selection activeCell="G735" sqref="G735"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -21867,6 +21867,267 @@
         <v>39</v>
       </c>
     </row>
+    <row r="734" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A734" t="s">
+        <v>9</v>
+      </c>
+      <c r="B734" s="3">
+        <v>111</v>
+      </c>
+      <c r="C734" t="s">
+        <v>20</v>
+      </c>
+      <c r="D734" s="3">
+        <v>99</v>
+      </c>
+      <c r="E734" t="s">
+        <v>67</v>
+      </c>
+      <c r="F734">
+        <v>17832</v>
+      </c>
+      <c r="G734" t="s">
+        <v>54</v>
+      </c>
+      <c r="H734" t="s">
+        <v>9</v>
+      </c>
+      <c r="I734" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="735" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A735" t="s">
+        <v>5</v>
+      </c>
+      <c r="B735" s="3">
+        <v>140</v>
+      </c>
+      <c r="C735" t="s">
+        <v>14</v>
+      </c>
+      <c r="D735" s="3">
+        <v>112</v>
+      </c>
+      <c r="E735" t="s">
+        <v>67</v>
+      </c>
+      <c r="F735">
+        <v>17832</v>
+      </c>
+      <c r="G735" t="s">
+        <v>55</v>
+      </c>
+      <c r="H735" t="s">
+        <v>5</v>
+      </c>
+      <c r="I735" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="736" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A736" t="s">
+        <v>30</v>
+      </c>
+      <c r="B736" s="3">
+        <v>91</v>
+      </c>
+      <c r="C736" t="s">
+        <v>11</v>
+      </c>
+      <c r="D736" s="3">
+        <v>131</v>
+      </c>
+      <c r="E736" t="s">
+        <v>67</v>
+      </c>
+      <c r="F736">
+        <v>17832</v>
+      </c>
+      <c r="G736" t="s">
+        <v>49</v>
+      </c>
+      <c r="H736" t="s">
+        <v>11</v>
+      </c>
+      <c r="I736" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="737" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A737" t="s">
+        <v>15</v>
+      </c>
+      <c r="B737" s="3">
+        <v>115</v>
+      </c>
+      <c r="C737" t="s">
+        <v>18</v>
+      </c>
+      <c r="D737" s="3">
+        <v>99</v>
+      </c>
+      <c r="E737" t="s">
+        <v>67</v>
+      </c>
+      <c r="F737">
+        <v>17832</v>
+      </c>
+      <c r="G737" t="s">
+        <v>19</v>
+      </c>
+      <c r="H737" t="s">
+        <v>15</v>
+      </c>
+      <c r="I737" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="738" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A738" t="s">
+        <v>42</v>
+      </c>
+      <c r="B738" s="3">
+        <v>103</v>
+      </c>
+      <c r="C738" t="s">
+        <v>21</v>
+      </c>
+      <c r="D738" s="3">
+        <v>95</v>
+      </c>
+      <c r="E738" t="s">
+        <v>67</v>
+      </c>
+      <c r="F738">
+        <v>17832</v>
+      </c>
+      <c r="G738" t="s">
+        <v>22</v>
+      </c>
+      <c r="H738" t="s">
+        <v>42</v>
+      </c>
+      <c r="I738" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="739" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A739" t="s">
+        <v>8</v>
+      </c>
+      <c r="B739" s="3">
+        <v>90</v>
+      </c>
+      <c r="C739" t="s">
+        <v>23</v>
+      </c>
+      <c r="D739" s="3">
+        <v>111</v>
+      </c>
+      <c r="E739" t="s">
+        <v>67</v>
+      </c>
+      <c r="F739">
+        <v>17832</v>
+      </c>
+      <c r="G739" t="s">
+        <v>57</v>
+      </c>
+      <c r="H739" t="s">
+        <v>23</v>
+      </c>
+      <c r="I739" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="740" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A740" t="s">
+        <v>24</v>
+      </c>
+      <c r="B740" s="3">
+        <v>127</v>
+      </c>
+      <c r="C740" t="s">
+        <v>32</v>
+      </c>
+      <c r="D740" s="3">
+        <v>135</v>
+      </c>
+      <c r="E740" t="s">
+        <v>67</v>
+      </c>
+      <c r="F740">
+        <v>17832</v>
+      </c>
+      <c r="G740" t="s">
+        <v>59</v>
+      </c>
+      <c r="H740" t="s">
+        <v>32</v>
+      </c>
+      <c r="I740" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="741" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A741" t="s">
+        <v>45</v>
+      </c>
+      <c r="B741" s="3">
+        <v>108</v>
+      </c>
+      <c r="C741" t="s">
+        <v>36</v>
+      </c>
+      <c r="D741" s="3">
+        <v>123</v>
+      </c>
+      <c r="E741" t="s">
+        <v>67</v>
+      </c>
+      <c r="F741">
+        <v>17832</v>
+      </c>
+      <c r="G741" t="s">
+        <v>37</v>
+      </c>
+      <c r="H741" t="s">
+        <v>36</v>
+      </c>
+      <c r="I741" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="742" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A742" t="s">
+        <v>41</v>
+      </c>
+      <c r="B742" s="3">
+        <v>103</v>
+      </c>
+      <c r="C742" t="s">
+        <v>3</v>
+      </c>
+      <c r="D742" s="3">
+        <v>112</v>
+      </c>
+      <c r="E742" t="s">
+        <v>67</v>
+      </c>
+      <c r="F742">
+        <v>17832</v>
+      </c>
+      <c r="G742" t="s">
+        <v>4</v>
+      </c>
+      <c r="H742" t="s">
+        <v>3</v>
+      </c>
+      <c r="I742" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified:   NBA2324.xlsx modified:   future.xlsx modified:   nba_forecast.ipynb modified:   nba_v1.1.ipynb
</commit_message>
<xml_diff>
--- a/NBA2324.xlsx
+++ b/NBA2324.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkdb\OneDrive\Desktop\ballgorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C056EF7-734E-407D-9F57-AD14100F5348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6288FD1D-3257-4BDC-9FEB-27A5648B3D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4533" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4575" uniqueCount="75">
   <si>
     <t>Attend.</t>
   </si>
@@ -592,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I755"/>
+  <dimension ref="A1:I762"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A722" workbookViewId="0">
-      <selection activeCell="H749" sqref="H749"/>
+    <sheetView tabSelected="1" topLeftCell="A729" workbookViewId="0">
+      <selection activeCell="G757" sqref="G757"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -22505,6 +22505,209 @@
         <v>45</v>
       </c>
     </row>
+    <row r="756" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A756" t="s">
+        <v>24</v>
+      </c>
+      <c r="B756" s="3">
+        <v>123</v>
+      </c>
+      <c r="C756" t="s">
+        <v>18</v>
+      </c>
+      <c r="D756" s="3">
+        <v>117</v>
+      </c>
+      <c r="E756" t="s">
+        <v>67</v>
+      </c>
+      <c r="F756">
+        <v>17832</v>
+      </c>
+      <c r="G756" t="s">
+        <v>19</v>
+      </c>
+      <c r="H756" t="s">
+        <v>24</v>
+      </c>
+      <c r="I756" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="757" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A757" t="s">
+        <v>26</v>
+      </c>
+      <c r="B757" s="3">
+        <v>114</v>
+      </c>
+      <c r="C757" t="s">
+        <v>14</v>
+      </c>
+      <c r="D757" s="3">
+        <v>106</v>
+      </c>
+      <c r="E757" t="s">
+        <v>67</v>
+      </c>
+      <c r="F757">
+        <v>17832</v>
+      </c>
+      <c r="G757" t="s">
+        <v>55</v>
+      </c>
+      <c r="H757" t="s">
+        <v>26</v>
+      </c>
+      <c r="I757" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="758" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A758" t="s">
+        <v>17</v>
+      </c>
+      <c r="B758" s="3">
+        <v>117</v>
+      </c>
+      <c r="C758" t="s">
+        <v>11</v>
+      </c>
+      <c r="D758" s="3">
+        <v>125</v>
+      </c>
+      <c r="E758" t="s">
+        <v>67</v>
+      </c>
+      <c r="F758">
+        <v>17832</v>
+      </c>
+      <c r="G758" t="s">
+        <v>49</v>
+      </c>
+      <c r="H758" t="s">
+        <v>11</v>
+      </c>
+      <c r="I758" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="759" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A759" t="s">
+        <v>39</v>
+      </c>
+      <c r="B759" s="3">
+        <v>104</v>
+      </c>
+      <c r="C759" t="s">
+        <v>21</v>
+      </c>
+      <c r="D759" s="3">
+        <v>116</v>
+      </c>
+      <c r="E759" t="s">
+        <v>67</v>
+      </c>
+      <c r="F759">
+        <v>17832</v>
+      </c>
+      <c r="G759" t="s">
+        <v>22</v>
+      </c>
+      <c r="H759" t="s">
+        <v>21</v>
+      </c>
+      <c r="I759" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="760" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A760" t="s">
+        <v>6</v>
+      </c>
+      <c r="B760" s="3">
+        <v>127</v>
+      </c>
+      <c r="C760" t="s">
+        <v>44</v>
+      </c>
+      <c r="D760" s="3">
+        <v>104</v>
+      </c>
+      <c r="E760" t="s">
+        <v>67</v>
+      </c>
+      <c r="F760">
+        <v>17832</v>
+      </c>
+      <c r="G760" t="s">
+        <v>61</v>
+      </c>
+      <c r="H760" t="s">
+        <v>6</v>
+      </c>
+      <c r="I760" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="761" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A761" t="s">
+        <v>29</v>
+      </c>
+      <c r="B761" s="3">
+        <v>117</v>
+      </c>
+      <c r="C761" t="s">
+        <v>42</v>
+      </c>
+      <c r="D761" s="3">
+        <v>106</v>
+      </c>
+      <c r="E761" t="s">
+        <v>67</v>
+      </c>
+      <c r="F761">
+        <v>17832</v>
+      </c>
+      <c r="G761" t="s">
+        <v>43</v>
+      </c>
+      <c r="H761" t="s">
+        <v>29</v>
+      </c>
+      <c r="I761" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="762" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A762" t="s">
+        <v>20</v>
+      </c>
+      <c r="B762" s="3">
+        <v>133</v>
+      </c>
+      <c r="C762" t="s">
+        <v>35</v>
+      </c>
+      <c r="D762" s="3">
+        <v>120</v>
+      </c>
+      <c r="E762" t="s">
+        <v>67</v>
+      </c>
+      <c r="F762">
+        <v>17832</v>
+      </c>
+      <c r="G762" t="s">
+        <v>53</v>
+      </c>
+      <c r="H762" t="s">
+        <v>20</v>
+      </c>
+      <c r="I762" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified:   NBA2324.xlsx modified:   cumulative_accuracy.ipynb modified:   espn_comparison.ipynb modified:   espn_comparison.xlsx new file:   excel_ballgorithm.xlsx modified:   future.xlsx modified:   nba_v1.1.ipynb
</commit_message>
<xml_diff>
--- a/NBA2324.xlsx
+++ b/NBA2324.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkdb\OneDrive\Desktop\ballgorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADECB831-248C-4CB0-B2CB-BDDE400FC474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7335E817-649E-4A7A-80FE-A0D13C8A4FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4629" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4665" uniqueCount="75">
   <si>
     <t>Attend.</t>
   </si>
@@ -592,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I771"/>
+  <dimension ref="A1:I777"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A739" workbookViewId="0">
-      <selection activeCell="G763" sqref="G763"/>
+    <sheetView tabSelected="1" topLeftCell="A744" workbookViewId="0">
+      <selection activeCell="G777" sqref="G777"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -22969,6 +22969,180 @@
         <v>41</v>
       </c>
     </row>
+    <row r="772" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A772" t="s">
+        <v>17</v>
+      </c>
+      <c r="B772" s="3">
+        <v>127</v>
+      </c>
+      <c r="C772" t="s">
+        <v>44</v>
+      </c>
+      <c r="D772" s="3">
+        <v>121</v>
+      </c>
+      <c r="E772" t="s">
+        <v>67</v>
+      </c>
+      <c r="F772">
+        <v>17832</v>
+      </c>
+      <c r="G772" t="s">
+        <v>61</v>
+      </c>
+      <c r="H772" t="s">
+        <v>17</v>
+      </c>
+      <c r="I772" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="773" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A773" t="s">
+        <v>14</v>
+      </c>
+      <c r="B773" s="3">
+        <v>129</v>
+      </c>
+      <c r="C773" t="s">
+        <v>11</v>
+      </c>
+      <c r="D773" s="3">
+        <v>133</v>
+      </c>
+      <c r="E773" t="s">
+        <v>67</v>
+      </c>
+      <c r="F773">
+        <v>17832</v>
+      </c>
+      <c r="G773" t="s">
+        <v>49</v>
+      </c>
+      <c r="H773" t="s">
+        <v>11</v>
+      </c>
+      <c r="I773" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="774" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A774" t="s">
+        <v>8</v>
+      </c>
+      <c r="B774" s="3">
+        <v>104</v>
+      </c>
+      <c r="C774" t="s">
+        <v>24</v>
+      </c>
+      <c r="D774" s="3">
+        <v>107</v>
+      </c>
+      <c r="E774" t="s">
+        <v>67</v>
+      </c>
+      <c r="F774">
+        <v>17832</v>
+      </c>
+      <c r="G774" t="s">
+        <v>25</v>
+      </c>
+      <c r="H774" t="s">
+        <v>24</v>
+      </c>
+      <c r="I774" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="775" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A775" t="s">
+        <v>18</v>
+      </c>
+      <c r="B775" s="3">
+        <v>84</v>
+      </c>
+      <c r="C775" t="s">
+        <v>45</v>
+      </c>
+      <c r="D775" s="3">
+        <v>120</v>
+      </c>
+      <c r="E775" t="s">
+        <v>67</v>
+      </c>
+      <c r="F775">
+        <v>17832</v>
+      </c>
+      <c r="G775" t="s">
+        <v>46</v>
+      </c>
+      <c r="H775" t="s">
+        <v>45</v>
+      </c>
+      <c r="I775" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="776" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A776" t="s">
+        <v>3</v>
+      </c>
+      <c r="B776" s="3">
+        <v>106</v>
+      </c>
+      <c r="C776" t="s">
+        <v>35</v>
+      </c>
+      <c r="D776" s="3">
+        <v>135</v>
+      </c>
+      <c r="E776" t="s">
+        <v>67</v>
+      </c>
+      <c r="F776">
+        <v>17832</v>
+      </c>
+      <c r="G776" t="s">
+        <v>53</v>
+      </c>
+      <c r="H776" t="s">
+        <v>35</v>
+      </c>
+      <c r="I776" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="777" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A777" t="s">
+        <v>29</v>
+      </c>
+      <c r="B777" s="3">
+        <v>122</v>
+      </c>
+      <c r="C777" t="s">
+        <v>2</v>
+      </c>
+      <c r="D777" s="3">
+        <v>139</v>
+      </c>
+      <c r="E777" t="s">
+        <v>67</v>
+      </c>
+      <c r="F777">
+        <v>17832</v>
+      </c>
+      <c r="G777" t="s">
+        <v>43</v>
+      </c>
+      <c r="H777" t="s">
+        <v>2</v>
+      </c>
+      <c r="I777" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified:   NBA2324.xlsx modified:   espn_comparison.ipynb modified:   espn_comparison.xlsx modified:   excel_ballgorithm.xlsx modified:   future.xlsx modified:   nba_v1.1.ipynb
</commit_message>
<xml_diff>
--- a/NBA2324.xlsx
+++ b/NBA2324.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkdb\OneDrive\Desktop\ballgorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7335E817-649E-4A7A-80FE-A0D13C8A4FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7073908-5836-4AC8-84DE-0218273BCC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4665" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4731" uniqueCount="75">
   <si>
     <t>Attend.</t>
   </si>
@@ -592,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I777"/>
+  <dimension ref="A1:I788"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A744" workbookViewId="0">
-      <selection activeCell="G777" sqref="G777"/>
+    <sheetView tabSelected="1" topLeftCell="A758" workbookViewId="0">
+      <selection activeCell="A778" sqref="A778"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -23143,6 +23143,325 @@
         <v>29</v>
       </c>
     </row>
+    <row r="778" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A778" t="s">
+        <v>32</v>
+      </c>
+      <c r="B778" s="3">
+        <v>111</v>
+      </c>
+      <c r="C778" t="s">
+        <v>38</v>
+      </c>
+      <c r="D778" s="3">
+        <v>146</v>
+      </c>
+      <c r="E778" t="s">
+        <v>67</v>
+      </c>
+      <c r="F778">
+        <v>17832</v>
+      </c>
+      <c r="G778" t="s">
+        <v>51</v>
+      </c>
+      <c r="H778" t="s">
+        <v>38</v>
+      </c>
+      <c r="I778" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="779" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A779" t="s">
+        <v>20</v>
+      </c>
+      <c r="B779" s="3">
+        <v>106</v>
+      </c>
+      <c r="C779" t="s">
+        <v>42</v>
+      </c>
+      <c r="D779" s="3">
+        <v>112</v>
+      </c>
+      <c r="E779" t="s">
+        <v>67</v>
+      </c>
+      <c r="F779">
+        <v>17832</v>
+      </c>
+      <c r="G779" t="s">
+        <v>43</v>
+      </c>
+      <c r="H779" t="s">
+        <v>42</v>
+      </c>
+      <c r="I779" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="780" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A780" t="s">
+        <v>39</v>
+      </c>
+      <c r="B780" s="3">
+        <v>103</v>
+      </c>
+      <c r="C780" t="s">
+        <v>27</v>
+      </c>
+      <c r="D780" s="3">
+        <v>123</v>
+      </c>
+      <c r="E780" t="s">
+        <v>67</v>
+      </c>
+      <c r="F780">
+        <v>17832</v>
+      </c>
+      <c r="G780" t="s">
+        <v>28</v>
+      </c>
+      <c r="H780" t="s">
+        <v>27</v>
+      </c>
+      <c r="I780" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="781" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A781" t="s">
+        <v>30</v>
+      </c>
+      <c r="B781" s="3">
+        <v>106</v>
+      </c>
+      <c r="C781" t="s">
+        <v>18</v>
+      </c>
+      <c r="D781" s="3">
+        <v>115</v>
+      </c>
+      <c r="E781" t="s">
+        <v>67</v>
+      </c>
+      <c r="F781">
+        <v>17832</v>
+      </c>
+      <c r="G781" t="s">
+        <v>19</v>
+      </c>
+      <c r="H781" t="s">
+        <v>18</v>
+      </c>
+      <c r="I781" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="782" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A782" t="s">
+        <v>33</v>
+      </c>
+      <c r="B782" s="3">
+        <v>108</v>
+      </c>
+      <c r="C782" t="s">
+        <v>9</v>
+      </c>
+      <c r="D782" s="3">
+        <v>114</v>
+      </c>
+      <c r="E782" t="s">
+        <v>67</v>
+      </c>
+      <c r="F782">
+        <v>17832</v>
+      </c>
+      <c r="G782" t="s">
+        <v>10</v>
+      </c>
+      <c r="H782" t="s">
+        <v>9</v>
+      </c>
+      <c r="I782" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="783" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A783" t="s">
+        <v>44</v>
+      </c>
+      <c r="B783" s="3">
+        <v>119</v>
+      </c>
+      <c r="C783" t="s">
+        <v>14</v>
+      </c>
+      <c r="D783" s="3">
+        <v>113</v>
+      </c>
+      <c r="E783" t="s">
+        <v>67</v>
+      </c>
+      <c r="F783">
+        <v>17832</v>
+      </c>
+      <c r="G783" t="s">
+        <v>55</v>
+      </c>
+      <c r="H783" t="s">
+        <v>44</v>
+      </c>
+      <c r="I783" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="784" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A784" t="s">
+        <v>8</v>
+      </c>
+      <c r="B784" s="3">
+        <v>113</v>
+      </c>
+      <c r="C784" t="s">
+        <v>17</v>
+      </c>
+      <c r="D784" s="3">
+        <v>122</v>
+      </c>
+      <c r="E784" t="s">
+        <v>67</v>
+      </c>
+      <c r="F784">
+        <v>17832</v>
+      </c>
+      <c r="G784" t="s">
+        <v>47</v>
+      </c>
+      <c r="H784" t="s">
+        <v>17</v>
+      </c>
+      <c r="I784" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="785" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A785" t="s">
+        <v>15</v>
+      </c>
+      <c r="B785" s="3">
+        <v>125</v>
+      </c>
+      <c r="C785" t="s">
+        <v>12</v>
+      </c>
+      <c r="D785" s="3">
+        <v>111</v>
+      </c>
+      <c r="E785" t="s">
+        <v>67</v>
+      </c>
+      <c r="F785">
+        <v>17832</v>
+      </c>
+      <c r="G785" t="s">
+        <v>13</v>
+      </c>
+      <c r="H785" t="s">
+        <v>15</v>
+      </c>
+      <c r="I785" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="786" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A786" t="s">
+        <v>26</v>
+      </c>
+      <c r="B786" s="3">
+        <v>119</v>
+      </c>
+      <c r="C786" t="s">
+        <v>24</v>
+      </c>
+      <c r="D786" s="3">
+        <v>95</v>
+      </c>
+      <c r="E786" t="s">
+        <v>67</v>
+      </c>
+      <c r="F786">
+        <v>17832</v>
+      </c>
+      <c r="G786" t="s">
+        <v>25</v>
+      </c>
+      <c r="H786" t="s">
+        <v>26</v>
+      </c>
+      <c r="I786" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="787" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A787" t="s">
+        <v>5</v>
+      </c>
+      <c r="B787" s="3">
+        <v>112</v>
+      </c>
+      <c r="C787" t="s">
+        <v>6</v>
+      </c>
+      <c r="D787" s="3">
+        <v>113</v>
+      </c>
+      <c r="E787" t="s">
+        <v>67</v>
+      </c>
+      <c r="F787">
+        <v>17832</v>
+      </c>
+      <c r="G787" t="s">
+        <v>7</v>
+      </c>
+      <c r="H787" t="s">
+        <v>6</v>
+      </c>
+      <c r="I787" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="788" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A788" t="s">
+        <v>29</v>
+      </c>
+      <c r="B788" s="3">
+        <v>93</v>
+      </c>
+      <c r="C788" t="s">
+        <v>41</v>
+      </c>
+      <c r="D788" s="3">
+        <v>84</v>
+      </c>
+      <c r="E788" t="s">
+        <v>67</v>
+      </c>
+      <c r="F788">
+        <v>17832</v>
+      </c>
+      <c r="G788" t="s">
+        <v>52</v>
+      </c>
+      <c r="H788" t="s">
+        <v>29</v>
+      </c>
+      <c r="I788" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified:   NBA2324.xlsx modified:   cumulative_accuracy.ipynb modified:   espn_comparison.ipynb modified:   espn_comparison.xlsx modified:   future.xlsx modified:   nba_v1.1.ipynb new file:   ven.ipynb
</commit_message>
<xml_diff>
--- a/NBA2324.xlsx
+++ b/NBA2324.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkdb\OneDrive\Desktop\ballgorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7073908-5836-4AC8-84DE-0218273BCC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E7FBFD-C9F0-4018-9289-9D6454F74509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4731" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4743" uniqueCount="75">
   <si>
     <t>Attend.</t>
   </si>
@@ -592,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I788"/>
+  <dimension ref="A1:I790"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A758" workbookViewId="0">
-      <selection activeCell="A778" sqref="A778"/>
+      <selection activeCell="H790" sqref="H790"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -23462,6 +23462,64 @@
         <v>41</v>
       </c>
     </row>
+    <row r="789" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A789" t="s">
+        <v>11</v>
+      </c>
+      <c r="B789" s="3">
+        <v>110</v>
+      </c>
+      <c r="C789" t="s">
+        <v>21</v>
+      </c>
+      <c r="D789" s="3">
+        <v>106</v>
+      </c>
+      <c r="E789" t="s">
+        <v>67</v>
+      </c>
+      <c r="F789">
+        <v>17832</v>
+      </c>
+      <c r="G789" t="s">
+        <v>22</v>
+      </c>
+      <c r="H789" t="s">
+        <v>11</v>
+      </c>
+      <c r="I789" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="790" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A790" t="s">
+        <v>35</v>
+      </c>
+      <c r="B790" s="3">
+        <v>113</v>
+      </c>
+      <c r="C790" t="s">
+        <v>32</v>
+      </c>
+      <c r="D790" s="3">
+        <v>127</v>
+      </c>
+      <c r="E790" t="s">
+        <v>67</v>
+      </c>
+      <c r="F790">
+        <v>17832</v>
+      </c>
+      <c r="G790" t="s">
+        <v>59</v>
+      </c>
+      <c r="H790" t="s">
+        <v>32</v>
+      </c>
+      <c r="I790" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified:   NBA2324.xlsx modified:   accuracy.ipynb modified:   cumulative_accuracy.ipynb modified:   espn_comparison.ipynb modified:   espn_comparison.xlsx modified:   future.xlsx modified:   nba_v1.1.ipynb
</commit_message>
<xml_diff>
--- a/NBA2324.xlsx
+++ b/NBA2324.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkdb\OneDrive\Desktop\ballgorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E7FBFD-C9F0-4018-9289-9D6454F74509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220EEC9F-C872-4D71-AEB7-1BDB3A771BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4743" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4803" uniqueCount="75">
   <si>
     <t>Attend.</t>
   </si>
@@ -592,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I790"/>
+  <dimension ref="A1:I800"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A758" workbookViewId="0">
-      <selection activeCell="H790" sqref="H790"/>
+    <sheetView tabSelected="1" topLeftCell="A770" workbookViewId="0">
+      <selection activeCell="A800" sqref="A800"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -23520,6 +23520,296 @@
         <v>35</v>
       </c>
     </row>
+    <row r="791" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A791" t="s">
+        <v>15</v>
+      </c>
+      <c r="B791" s="3">
+        <v>102</v>
+      </c>
+      <c r="C791" t="s">
+        <v>18</v>
+      </c>
+      <c r="D791" s="3">
+        <v>111</v>
+      </c>
+      <c r="E791" t="s">
+        <v>67</v>
+      </c>
+      <c r="F791">
+        <v>17832</v>
+      </c>
+      <c r="G791" t="s">
+        <v>19</v>
+      </c>
+      <c r="H791" t="s">
+        <v>18</v>
+      </c>
+      <c r="I791" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="792" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A792" t="s">
+        <v>44</v>
+      </c>
+      <c r="B792" s="3">
+        <v>123</v>
+      </c>
+      <c r="C792" t="s">
+        <v>26</v>
+      </c>
+      <c r="D792" s="3">
+        <v>121</v>
+      </c>
+      <c r="E792" t="s">
+        <v>67</v>
+      </c>
+      <c r="F792">
+        <v>17832</v>
+      </c>
+      <c r="G792" t="s">
+        <v>48</v>
+      </c>
+      <c r="H792" t="s">
+        <v>44</v>
+      </c>
+      <c r="I792" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="793" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A793" t="s">
+        <v>33</v>
+      </c>
+      <c r="B793" s="3">
+        <v>136</v>
+      </c>
+      <c r="C793" t="s">
+        <v>17</v>
+      </c>
+      <c r="D793" s="3">
+        <v>126</v>
+      </c>
+      <c r="E793" t="s">
+        <v>67</v>
+      </c>
+      <c r="F793">
+        <v>17832</v>
+      </c>
+      <c r="G793" t="s">
+        <v>47</v>
+      </c>
+      <c r="H793" t="s">
+        <v>33</v>
+      </c>
+      <c r="I793" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="794" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A794" t="s">
+        <v>39</v>
+      </c>
+      <c r="B794" s="3">
+        <v>122</v>
+      </c>
+      <c r="C794" t="s">
+        <v>24</v>
+      </c>
+      <c r="D794" s="3">
+        <v>99</v>
+      </c>
+      <c r="E794" t="s">
+        <v>67</v>
+      </c>
+      <c r="F794">
+        <v>17832</v>
+      </c>
+      <c r="G794" t="s">
+        <v>25</v>
+      </c>
+      <c r="H794" t="s">
+        <v>39</v>
+      </c>
+      <c r="I794" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="795" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A795" t="s">
+        <v>12</v>
+      </c>
+      <c r="B795" s="3">
+        <v>103</v>
+      </c>
+      <c r="C795" t="s">
+        <v>8</v>
+      </c>
+      <c r="D795" s="3">
+        <v>105</v>
+      </c>
+      <c r="E795" t="s">
+        <v>67</v>
+      </c>
+      <c r="F795">
+        <v>17832</v>
+      </c>
+      <c r="G795" t="s">
+        <v>60</v>
+      </c>
+      <c r="H795" t="s">
+        <v>8</v>
+      </c>
+      <c r="I795" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="796" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A796" t="s">
+        <v>29</v>
+      </c>
+      <c r="B796" s="3">
+        <v>96</v>
+      </c>
+      <c r="C796" t="s">
+        <v>30</v>
+      </c>
+      <c r="D796" s="3">
+        <v>87</v>
+      </c>
+      <c r="E796" t="s">
+        <v>67</v>
+      </c>
+      <c r="F796">
+        <v>17832</v>
+      </c>
+      <c r="G796" t="s">
+        <v>31</v>
+      </c>
+      <c r="H796" t="s">
+        <v>29</v>
+      </c>
+      <c r="I796" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="797" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A797" t="s">
+        <v>3</v>
+      </c>
+      <c r="B797" s="3">
+        <v>95</v>
+      </c>
+      <c r="C797" t="s">
+        <v>45</v>
+      </c>
+      <c r="D797" s="3">
+        <v>112</v>
+      </c>
+      <c r="E797" t="s">
+        <v>67</v>
+      </c>
+      <c r="F797">
+        <v>17832</v>
+      </c>
+      <c r="G797" t="s">
+        <v>46</v>
+      </c>
+      <c r="H797" t="s">
+        <v>45</v>
+      </c>
+      <c r="I797" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="798" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A798" t="s">
+        <v>14</v>
+      </c>
+      <c r="B798" s="3">
+        <v>104</v>
+      </c>
+      <c r="C798" t="s">
+        <v>38</v>
+      </c>
+      <c r="D798" s="3">
+        <v>112</v>
+      </c>
+      <c r="E798" t="s">
+        <v>67</v>
+      </c>
+      <c r="F798">
+        <v>17832</v>
+      </c>
+      <c r="G798" t="s">
+        <v>51</v>
+      </c>
+      <c r="H798" t="s">
+        <v>38</v>
+      </c>
+      <c r="I798" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="799" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A799" t="s">
+        <v>6</v>
+      </c>
+      <c r="B799" s="3">
+        <v>129</v>
+      </c>
+      <c r="C799" t="s">
+        <v>36</v>
+      </c>
+      <c r="D799" s="3">
+        <v>107</v>
+      </c>
+      <c r="E799" t="s">
+        <v>67</v>
+      </c>
+      <c r="F799">
+        <v>17832</v>
+      </c>
+      <c r="G799" t="s">
+        <v>37</v>
+      </c>
+      <c r="H799" t="s">
+        <v>6</v>
+      </c>
+      <c r="I799" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="800" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A800" t="s">
+        <v>23</v>
+      </c>
+      <c r="B800" s="3">
+        <v>121</v>
+      </c>
+      <c r="C800" t="s">
+        <v>42</v>
+      </c>
+      <c r="D800" s="3">
+        <v>100</v>
+      </c>
+      <c r="E800" t="s">
+        <v>67</v>
+      </c>
+      <c r="F800">
+        <v>17832</v>
+      </c>
+      <c r="G800" t="s">
+        <v>43</v>
+      </c>
+      <c r="H800" t="s">
+        <v>23</v>
+      </c>
+      <c r="I800" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified:   NBA2324.xlsx modified:   espn_comparison.ipynb modified:   espn_comparison.xlsx modified:   future.xlsx modified:   nba_v1.1.ipynb
</commit_message>
<xml_diff>
--- a/NBA2324.xlsx
+++ b/NBA2324.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkdb\OneDrive\Desktop\ballgorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EE4977-7EA4-4D33-AED5-F26D34100049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB003D57-2B4E-4FEB-B868-7A7568DEDD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4904" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4935" uniqueCount="75">
   <si>
     <t>Attend.</t>
   </si>
@@ -592,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I819"/>
+  <dimension ref="A1:I822"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A787" workbookViewId="0">
-      <selection activeCell="F808" sqref="F808"/>
+    <sheetView tabSelected="1" topLeftCell="A791" workbookViewId="0">
+      <selection activeCell="A821" sqref="A821"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -23997,6 +23997,9 @@
       <c r="D807">
         <v>122</v>
       </c>
+      <c r="E807" t="s">
+        <v>67</v>
+      </c>
       <c r="F807">
         <v>17832</v>
       </c>
@@ -24023,6 +24026,9 @@
       <c r="D808">
         <v>118</v>
       </c>
+      <c r="E808" t="s">
+        <v>67</v>
+      </c>
       <c r="F808">
         <v>17832</v>
       </c>
@@ -24049,6 +24055,9 @@
       <c r="D809">
         <v>104</v>
       </c>
+      <c r="E809" t="s">
+        <v>67</v>
+      </c>
       <c r="F809">
         <v>17832</v>
       </c>
@@ -24075,6 +24084,9 @@
       <c r="D810">
         <v>136</v>
       </c>
+      <c r="E810" t="s">
+        <v>67</v>
+      </c>
       <c r="F810">
         <v>17832</v>
       </c>
@@ -24101,6 +24113,9 @@
       <c r="D811">
         <v>108</v>
       </c>
+      <c r="E811" t="s">
+        <v>67</v>
+      </c>
       <c r="F811">
         <v>17832</v>
       </c>
@@ -24127,6 +24142,9 @@
       <c r="D812">
         <v>125</v>
       </c>
+      <c r="E812" t="s">
+        <v>67</v>
+      </c>
       <c r="F812">
         <v>17832</v>
       </c>
@@ -24153,6 +24171,9 @@
       <c r="D813">
         <v>121</v>
       </c>
+      <c r="E813" t="s">
+        <v>67</v>
+      </c>
       <c r="F813">
         <v>17832</v>
       </c>
@@ -24179,6 +24200,9 @@
       <c r="D814">
         <v>133</v>
       </c>
+      <c r="E814" t="s">
+        <v>67</v>
+      </c>
       <c r="F814">
         <v>17832</v>
       </c>
@@ -24205,6 +24229,9 @@
       <c r="D815">
         <v>116</v>
       </c>
+      <c r="E815" t="s">
+        <v>67</v>
+      </c>
       <c r="F815">
         <v>17832</v>
       </c>
@@ -24231,6 +24258,9 @@
       <c r="D816">
         <v>98</v>
       </c>
+      <c r="E816" t="s">
+        <v>67</v>
+      </c>
       <c r="F816">
         <v>17832</v>
       </c>
@@ -24257,6 +24287,9 @@
       <c r="D817">
         <v>116</v>
       </c>
+      <c r="E817" t="s">
+        <v>67</v>
+      </c>
       <c r="F817">
         <v>17832</v>
       </c>
@@ -24283,6 +24316,9 @@
       <c r="D818">
         <v>122</v>
       </c>
+      <c r="E818" t="s">
+        <v>67</v>
+      </c>
       <c r="F818">
         <v>17832</v>
       </c>
@@ -24309,6 +24345,9 @@
       <c r="D819">
         <v>125</v>
       </c>
+      <c r="E819" t="s">
+        <v>67</v>
+      </c>
       <c r="F819">
         <v>17832</v>
       </c>
@@ -24320,6 +24359,93 @@
       </c>
       <c r="I819" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="820" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A820" t="s">
+        <v>45</v>
+      </c>
+      <c r="B820">
+        <v>110</v>
+      </c>
+      <c r="C820" t="s">
+        <v>30</v>
+      </c>
+      <c r="D820">
+        <v>113</v>
+      </c>
+      <c r="E820" t="s">
+        <v>67</v>
+      </c>
+      <c r="F820">
+        <v>17832</v>
+      </c>
+      <c r="G820" t="s">
+        <v>31</v>
+      </c>
+      <c r="H820" t="s">
+        <v>30</v>
+      </c>
+      <c r="I820" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="821" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A821" t="s">
+        <v>6</v>
+      </c>
+      <c r="B821">
+        <v>140</v>
+      </c>
+      <c r="C821" t="s">
+        <v>36</v>
+      </c>
+      <c r="D821">
+        <v>137</v>
+      </c>
+      <c r="E821" t="s">
+        <v>67</v>
+      </c>
+      <c r="F821">
+        <v>17832</v>
+      </c>
+      <c r="G821" t="s">
+        <v>37</v>
+      </c>
+      <c r="H821" t="s">
+        <v>6</v>
+      </c>
+      <c r="I821" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="822" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A822" t="s">
+        <v>23</v>
+      </c>
+      <c r="B822">
+        <v>128</v>
+      </c>
+      <c r="C822" t="s">
+        <v>41</v>
+      </c>
+      <c r="D822">
+        <v>91</v>
+      </c>
+      <c r="E822" t="s">
+        <v>67</v>
+      </c>
+      <c r="F822">
+        <v>17832</v>
+      </c>
+      <c r="G822" t="s">
+        <v>52</v>
+      </c>
+      <c r="H822" t="s">
+        <v>23</v>
+      </c>
+      <c r="I822" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   NBA2324.xlsx new file:   desktop.ini modified:   espn_comparison.ipynb modified:   espn_comparison.xlsx modified:   future.xlsx modified:   nba_v1.1.ipynb
</commit_message>
<xml_diff>
--- a/NBA2324.xlsx
+++ b/NBA2324.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkdb\OneDrive\Desktop\ballgorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE3B44D-35C7-4CCE-9E1F-EFC4B7AA8971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5DE457-E810-4115-AC38-D61E5515BF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5067" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5085" uniqueCount="75">
   <si>
     <t>Attend.</t>
   </si>
@@ -592,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I844"/>
+  <dimension ref="A1:I847"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A812" workbookViewId="0">
-      <selection activeCell="G835" sqref="G835"/>
+    <sheetView tabSelected="1" topLeftCell="A815" workbookViewId="0">
+      <selection activeCell="G845" sqref="G845"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -25086,6 +25086,93 @@
         <v>39</v>
       </c>
     </row>
+    <row r="845" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A845" t="s">
+        <v>9</v>
+      </c>
+      <c r="B845">
+        <v>112</v>
+      </c>
+      <c r="C845" t="s">
+        <v>20</v>
+      </c>
+      <c r="D845">
+        <v>109</v>
+      </c>
+      <c r="E845" t="s">
+        <v>67</v>
+      </c>
+      <c r="F845">
+        <v>17832</v>
+      </c>
+      <c r="G845" t="s">
+        <v>54</v>
+      </c>
+      <c r="H845" t="s">
+        <v>9</v>
+      </c>
+      <c r="I845" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="846" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A846" t="s">
+        <v>11</v>
+      </c>
+      <c r="B846">
+        <v>116</v>
+      </c>
+      <c r="C846" t="s">
+        <v>12</v>
+      </c>
+      <c r="D846">
+        <v>102</v>
+      </c>
+      <c r="E846" t="s">
+        <v>67</v>
+      </c>
+      <c r="F846">
+        <v>17832</v>
+      </c>
+      <c r="G846" t="s">
+        <v>13</v>
+      </c>
+      <c r="H846" t="s">
+        <v>11</v>
+      </c>
+      <c r="I846" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="847" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A847" t="s">
+        <v>27</v>
+      </c>
+      <c r="B847">
+        <v>86</v>
+      </c>
+      <c r="C847" t="s">
+        <v>23</v>
+      </c>
+      <c r="D847">
+        <v>101</v>
+      </c>
+      <c r="E847" t="s">
+        <v>67</v>
+      </c>
+      <c r="F847">
+        <v>17832</v>
+      </c>
+      <c r="G847" t="s">
+        <v>57</v>
+      </c>
+      <c r="H847" t="s">
+        <v>23</v>
+      </c>
+      <c r="I847" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified:   NBA2324.xlsx modified:   future.xlsx modified:   nba_v1.1.ipynb
</commit_message>
<xml_diff>
--- a/NBA2324.xlsx
+++ b/NBA2324.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkdb\OneDrive\Desktop\ballgorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990AACC8-7B5F-4770-8DA8-24ADA6D48384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEBE9BC-B085-4523-B698-9FCF5A2E532F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5595" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5685" uniqueCount="75">
   <si>
     <t>Attend.</t>
   </si>
@@ -592,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I932"/>
+  <dimension ref="A1:I947"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A900" workbookViewId="0">
-      <selection activeCell="G925" sqref="G925"/>
+    <sheetView tabSelected="1" topLeftCell="A916" workbookViewId="0">
+      <selection activeCell="A947" sqref="A947"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -27638,6 +27638,441 @@
         <v>2</v>
       </c>
     </row>
+    <row r="933" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A933" t="s">
+        <v>27</v>
+      </c>
+      <c r="B933">
+        <v>112</v>
+      </c>
+      <c r="C933" t="s">
+        <v>20</v>
+      </c>
+      <c r="D933">
+        <v>118</v>
+      </c>
+      <c r="E933" t="s">
+        <v>67</v>
+      </c>
+      <c r="F933">
+        <v>17832</v>
+      </c>
+      <c r="G933" t="s">
+        <v>54</v>
+      </c>
+      <c r="H933" t="s">
+        <v>20</v>
+      </c>
+      <c r="I933" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="934" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A934" t="s">
+        <v>23</v>
+      </c>
+      <c r="B934">
+        <v>113</v>
+      </c>
+      <c r="C934" t="s">
+        <v>15</v>
+      </c>
+      <c r="D934">
+        <v>111</v>
+      </c>
+      <c r="E934" t="s">
+        <v>67</v>
+      </c>
+      <c r="F934">
+        <v>17832</v>
+      </c>
+      <c r="G934" t="s">
+        <v>16</v>
+      </c>
+      <c r="H934" t="s">
+        <v>23</v>
+      </c>
+      <c r="I934" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="935" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A935" t="s">
+        <v>21</v>
+      </c>
+      <c r="B935">
+        <v>108</v>
+      </c>
+      <c r="C935" t="s">
+        <v>38</v>
+      </c>
+      <c r="D935">
+        <v>114</v>
+      </c>
+      <c r="E935" t="s">
+        <v>67</v>
+      </c>
+      <c r="F935">
+        <v>17832</v>
+      </c>
+      <c r="G935" t="s">
+        <v>51</v>
+      </c>
+      <c r="H935" t="s">
+        <v>38</v>
+      </c>
+      <c r="I935" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="936" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A936" t="s">
+        <v>24</v>
+      </c>
+      <c r="B936">
+        <v>113</v>
+      </c>
+      <c r="C936" t="s">
+        <v>5</v>
+      </c>
+      <c r="D936">
+        <v>120</v>
+      </c>
+      <c r="E936" t="s">
+        <v>67</v>
+      </c>
+      <c r="F936">
+        <v>17832</v>
+      </c>
+      <c r="G936" t="s">
+        <v>58</v>
+      </c>
+      <c r="H936" t="s">
+        <v>5</v>
+      </c>
+      <c r="I936" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="937" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A937" t="s">
+        <v>11</v>
+      </c>
+      <c r="B937">
+        <v>109</v>
+      </c>
+      <c r="C937" t="s">
+        <v>3</v>
+      </c>
+      <c r="D937">
+        <v>115</v>
+      </c>
+      <c r="E937" t="s">
+        <v>67</v>
+      </c>
+      <c r="F937">
+        <v>17832</v>
+      </c>
+      <c r="G937" t="s">
+        <v>4</v>
+      </c>
+      <c r="H937" t="s">
+        <v>3</v>
+      </c>
+      <c r="I937" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="938" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A938" t="s">
+        <v>33</v>
+      </c>
+      <c r="B938">
+        <v>125</v>
+      </c>
+      <c r="C938" t="s">
+        <v>6</v>
+      </c>
+      <c r="D938">
+        <v>122</v>
+      </c>
+      <c r="E938" t="s">
+        <v>67</v>
+      </c>
+      <c r="F938">
+        <v>17832</v>
+      </c>
+      <c r="G938" t="s">
+        <v>7</v>
+      </c>
+      <c r="H938" t="s">
+        <v>33</v>
+      </c>
+      <c r="I938" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="939" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A939" t="s">
+        <v>39</v>
+      </c>
+      <c r="B939">
+        <v>129</v>
+      </c>
+      <c r="C939" t="s">
+        <v>35</v>
+      </c>
+      <c r="D939">
+        <v>131</v>
+      </c>
+      <c r="E939" t="s">
+        <v>67</v>
+      </c>
+      <c r="F939">
+        <v>17832</v>
+      </c>
+      <c r="G939" t="s">
+        <v>53</v>
+      </c>
+      <c r="H939" t="s">
+        <v>35</v>
+      </c>
+      <c r="I939" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="940" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A940" t="s">
+        <v>29</v>
+      </c>
+      <c r="B940">
+        <v>103</v>
+      </c>
+      <c r="C940" t="s">
+        <v>44</v>
+      </c>
+      <c r="D940">
+        <v>95</v>
+      </c>
+      <c r="E940" t="s">
+        <v>67</v>
+      </c>
+      <c r="F940">
+        <v>17832</v>
+      </c>
+      <c r="G940" t="s">
+        <v>61</v>
+      </c>
+      <c r="H940" t="s">
+        <v>29</v>
+      </c>
+      <c r="I940" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="941" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A941" t="s">
+        <v>18</v>
+      </c>
+      <c r="B941">
+        <v>100</v>
+      </c>
+      <c r="C941" t="s">
+        <v>14</v>
+      </c>
+      <c r="D941">
+        <v>112</v>
+      </c>
+      <c r="E941" t="s">
+        <v>67</v>
+      </c>
+      <c r="F941">
+        <v>17832</v>
+      </c>
+      <c r="G941" t="s">
+        <v>55</v>
+      </c>
+      <c r="H941" t="s">
+        <v>14</v>
+      </c>
+      <c r="I941" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="942" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A942" t="s">
+        <v>23</v>
+      </c>
+      <c r="B942">
+        <v>104</v>
+      </c>
+      <c r="C942" t="s">
+        <v>26</v>
+      </c>
+      <c r="D942">
+        <v>113</v>
+      </c>
+      <c r="E942" t="s">
+        <v>50</v>
+      </c>
+      <c r="F942">
+        <v>17832</v>
+      </c>
+      <c r="G942" t="s">
+        <v>48</v>
+      </c>
+      <c r="H942" t="s">
+        <v>26</v>
+      </c>
+      <c r="I942" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="943" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A943" t="s">
+        <v>9</v>
+      </c>
+      <c r="B943">
+        <v>74</v>
+      </c>
+      <c r="C943" t="s">
+        <v>12</v>
+      </c>
+      <c r="D943">
+        <v>98</v>
+      </c>
+      <c r="E943" t="s">
+        <v>67</v>
+      </c>
+      <c r="F943">
+        <v>17832</v>
+      </c>
+      <c r="G943" t="s">
+        <v>13</v>
+      </c>
+      <c r="H943" t="s">
+        <v>12</v>
+      </c>
+      <c r="I943" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="944" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A944" t="s">
+        <v>17</v>
+      </c>
+      <c r="B944">
+        <v>99</v>
+      </c>
+      <c r="C944" t="s">
+        <v>30</v>
+      </c>
+      <c r="D944">
+        <v>92</v>
+      </c>
+      <c r="E944" t="s">
+        <v>67</v>
+      </c>
+      <c r="F944">
+        <v>17832</v>
+      </c>
+      <c r="G944" t="s">
+        <v>31</v>
+      </c>
+      <c r="H944" t="s">
+        <v>17</v>
+      </c>
+      <c r="I944" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="945" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A945" t="s">
+        <v>21</v>
+      </c>
+      <c r="B945">
+        <v>100</v>
+      </c>
+      <c r="C945" t="s">
+        <v>32</v>
+      </c>
+      <c r="D945">
+        <v>107</v>
+      </c>
+      <c r="E945" t="s">
+        <v>67</v>
+      </c>
+      <c r="F945">
+        <v>17832</v>
+      </c>
+      <c r="G945" t="s">
+        <v>59</v>
+      </c>
+      <c r="H945" t="s">
+        <v>32</v>
+      </c>
+      <c r="I945" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="946" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A946" t="s">
+        <v>45</v>
+      </c>
+      <c r="B946">
+        <v>122</v>
+      </c>
+      <c r="C946" t="s">
+        <v>2</v>
+      </c>
+      <c r="D946">
+        <v>123</v>
+      </c>
+      <c r="E946" t="s">
+        <v>67</v>
+      </c>
+      <c r="F946">
+        <v>17832</v>
+      </c>
+      <c r="G946" t="s">
+        <v>43</v>
+      </c>
+      <c r="H946" t="s">
+        <v>2</v>
+      </c>
+      <c r="I946" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="947" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A947" t="s">
+        <v>8</v>
+      </c>
+      <c r="B947">
+        <v>123</v>
+      </c>
+      <c r="C947" t="s">
+        <v>41</v>
+      </c>
+      <c r="D947">
+        <v>107</v>
+      </c>
+      <c r="E947" t="s">
+        <v>67</v>
+      </c>
+      <c r="F947">
+        <v>17832</v>
+      </c>
+      <c r="G947" t="s">
+        <v>52</v>
+      </c>
+      <c r="H947" t="s">
+        <v>8</v>
+      </c>
+      <c r="I947" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>